<commit_message>
Working prototype of front-end and improved python documentation
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
-  <si>
-    <t>DUTY 110724 THURSDAY</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+  <si>
+    <t>DUTY 210724 SUNDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -61,36 +61,39 @@
     <t>HAKIM</t>
   </si>
   <si>
+    <t>SCA1</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
     <t>IN</t>
   </si>
   <si>
-    <t>OUT</t>
-  </si>
-  <si>
     <t>SENTRY</t>
   </si>
   <si>
     <t>XAVIER</t>
   </si>
   <si>
+    <t>SCA2</t>
+  </si>
+  <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
     <t>X-RAY</t>
   </si>
   <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
     <t>TAN DI ER</t>
   </si>
   <si>
+    <t>ANIQ</t>
+  </si>
+  <si>
     <t>DESK</t>
   </si>
   <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
-    <t>SCA1</t>
-  </si>
-  <si>
     <t>JUN</t>
   </si>
   <si>
@@ -100,6 +103,9 @@
     <t>JOSHUA</t>
   </si>
   <si>
+    <t>AL</t>
+  </si>
+  <si>
     <t>ANIISH</t>
   </si>
   <si>
@@ -112,22 +118,19 @@
     <t>DHRUVA</t>
   </si>
   <si>
-    <t>SCA2</t>
+    <t>PAC</t>
   </si>
   <si>
     <t>MARC</t>
   </si>
   <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>FLAG:HAKIM // TAN DI ER // SYAFI'I</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: ANIQ</t>
-  </si>
-  <si>
-    <t>BREAKFAST:JUN // DINNER:TAN DI ER</t>
+    <t>FLAG:XAVIER // MARC // TAN DI ER</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: HILMI</t>
+  </si>
+  <si>
+    <t>BREAKFAST:MARC // DINNER:JUN</t>
   </si>
 </sst>
 </file>
@@ -188,6 +191,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -207,12 +216,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,12 +273,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -294,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -669,26 +672,28 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="K3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -697,28 +702,26 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="4">
         <v>6</v>
       </c>
@@ -729,28 +732,30 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="L7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="9"/>
       <c r="N7" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -759,26 +764,28 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="9" t="s">
+      <c r="H9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="4">
         <v>6</v>
       </c>
@@ -789,32 +796,32 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="7"/>
       <c r="N11" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -823,32 +830,32 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="M13" s="10"/>
       <c r="N13" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -857,32 +864,34 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="8"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -891,32 +900,24 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
       <c r="N17" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -925,10 +926,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -951,30 +952,30 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="5" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="F21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="4">
         <v>6</v>
       </c>
@@ -985,30 +986,34 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="12"/>
       <c r="N23" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1017,42 +1022,42 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="12"/>
+      <c r="H25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -1061,7 +1066,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -1100,24 +1105,25 @@
       <c r="N28" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="B17:M17"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>
     <mergeCell ref="D26:J28"/>

</xml_diff>

<commit_message>
Working calendar UI for displaying and editing events
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 210724 SUNDAY</t>
+    <t>DUTY 250724 THURSDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -64,42 +64,45 @@
     <t>SCA1</t>
   </si>
   <si>
+    <t>SENTRY</t>
+  </si>
+  <si>
+    <t>X-RAY</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>OUT</t>
   </si>
   <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>SENTRY</t>
-  </si>
-  <si>
-    <t>XAVIER</t>
+    <t>KAH FAI</t>
   </si>
   <si>
     <t>SCA2</t>
   </si>
   <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>X-RAY</t>
-  </si>
-  <si>
     <t>TAN DI ER</t>
   </si>
   <si>
+    <t>DESK</t>
+  </si>
+  <si>
     <t>ANIQ</t>
   </si>
   <si>
-    <t>DESK</t>
-  </si>
-  <si>
     <t>JUN</t>
   </si>
   <si>
     <t>SYAFI'I</t>
   </si>
   <si>
+    <t>PAC</t>
+  </si>
+  <si>
     <t>JOSHUA</t>
   </si>
   <si>
@@ -118,19 +121,16 @@
     <t>DHRUVA</t>
   </si>
   <si>
-    <t>PAC</t>
-  </si>
-  <si>
     <t>MARC</t>
   </si>
   <si>
-    <t>FLAG:XAVIER // MARC // TAN DI ER</t>
+    <t>FLAG:MARC // XAVIER // SYAFI'I</t>
   </si>
   <si>
     <t>LAST ENSURER: HILMI</t>
   </si>
   <si>
-    <t>BREAKFAST:MARC // DINNER:JUN</t>
+    <t>BREAKFAST:JUN // DINNER:SYAFI'I</t>
   </si>
 </sst>
 </file>
@@ -197,12 +197,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -215,19 +209,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
+        <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FF999999"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,10 +291,10 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,23 +677,21 @@
         <v>15</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
       <c r="N3" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -702,22 +700,24 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -735,25 +735,25 @@
         <v>21</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="K7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="4">
         <v>7</v>
       </c>
@@ -766,28 +766,28 @@
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="F9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="10"/>
       <c r="N9" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -796,30 +796,30 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="7"/>
+      <c r="L11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="4"/>
       <c r="N11" s="4">
         <v>7</v>
       </c>
@@ -832,28 +832,28 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>17</v>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="10"/>
+      <c r="K13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="9"/>
       <c r="N13" s="4">
         <v>7</v>
       </c>
@@ -870,26 +870,26 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>17</v>
+      <c r="H15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="11"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -900,22 +900,22 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
       <c r="N17" s="4">
         <v>0</v>
       </c>
@@ -926,22 +926,22 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="B19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="4">
         <v>0</v>
       </c>
@@ -952,23 +952,23 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -986,32 +986,32 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="10" t="s">
-        <v>25</v>
+      <c r="F23" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="8"/>
       <c r="N23" s="4">
         <v>7</v>
       </c>
@@ -1024,22 +1024,22 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="10" t="s">
-        <v>25</v>
+      <c r="B25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1108,12 +1108,12 @@
   <mergeCells count="21">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="L9:M9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="B13:C13"/>

</xml_diff>

<commit_message>
Added draggables corresponding to the roles and demo the flow of data with eel
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 250724 THURSDAY</t>
+    <t>DUTY 300724 TUESDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -67,42 +67,42 @@
     <t>SENTRY</t>
   </si>
   <si>
+    <t>DESK</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>X-RAY</t>
   </si>
   <si>
-    <t>XAVIER</t>
-  </si>
-  <si>
-    <t>IN</t>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>TAN DI ER</t>
   </si>
   <si>
     <t>OUT</t>
   </si>
   <si>
-    <t>KAH FAI</t>
+    <t>ANIQ</t>
   </si>
   <si>
     <t>SCA2</t>
   </si>
   <si>
-    <t>TAN DI ER</t>
-  </si>
-  <si>
-    <t>DESK</t>
-  </si>
-  <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
     <t>JUN</t>
   </si>
   <si>
     <t>SYAFI'I</t>
   </si>
   <si>
-    <t>PAC</t>
-  </si>
-  <si>
     <t>JOSHUA</t>
   </si>
   <si>
@@ -124,13 +124,13 @@
     <t>MARC</t>
   </si>
   <si>
-    <t>FLAG:MARC // XAVIER // SYAFI'I</t>
+    <t>FLAG:TAN DI ER // DHRUVA // SYAFI'I</t>
   </si>
   <si>
     <t>LAST ENSURER: HILMI</t>
   </si>
   <si>
-    <t>BREAKFAST:JUN // DINNER:SYAFI'I</t>
+    <t>BREAKFAST:DHRUVA // DINNER:JUN</t>
   </si>
 </sst>
 </file>
@@ -203,7 +203,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +215,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
+        <fgColor rgb="FF00FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -709,14 +709,14 @@
       <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="10" t="s">
         <v>20</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -735,25 +735,25 @@
         <v>21</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="4">
         <v>7</v>
       </c>
@@ -770,22 +770,24 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="10"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="4">
         <v>7</v>
       </c>
@@ -798,26 +800,26 @@
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9" t="s">
-        <v>19</v>
+      <c r="I11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4">
@@ -830,30 +832,30 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="8" t="s">
+      <c r="J13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="4">
         <v>7</v>
       </c>
@@ -864,32 +866,32 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="11"/>
+      <c r="M15" s="10"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -954,21 +956,21 @@
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -988,32 +990,30 @@
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="9" t="s">
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="F23" s="5"/>
       <c r="G23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="8"/>
+      <c r="H23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1024,30 +1024,30 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="B25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="K25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="9"/>
       <c r="N25" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1110,11 +1110,10 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="L13:M13"/>
@@ -1122,8 +1121,9 @@
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B25:C25"/>
+    <mergeCell ref="L25:M25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>
     <mergeCell ref="D26:J28"/>

</xml_diff>

<commit_message>
Successfully implemented until generate specific duty
TODO: Update the miscellaneous roles, make hours change dynamically
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 010824 THURSDAY</t>
+    <t>DUTY 060824 TUESDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -61,42 +61,45 @@
     <t>HAKIM</t>
   </si>
   <si>
+    <t>SENTRY</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>X-RAY</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
+    <t>SCA1</t>
+  </si>
+  <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>SCA2</t>
+  </si>
+  <si>
     <t>DESK</t>
   </si>
   <si>
-    <t>SENTRY</t>
-  </si>
-  <si>
-    <t>X-RAY</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>XAVIER</t>
-  </si>
-  <si>
-    <t>SCA1</t>
-  </si>
-  <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
     <t>TAN DI ER</t>
   </si>
   <si>
-    <t>SCA2</t>
-  </si>
-  <si>
     <t>ANIQ</t>
   </si>
   <si>
     <t>JUN</t>
   </si>
   <si>
+    <t>PAC</t>
+  </si>
+  <si>
     <t>SYAFI'I</t>
   </si>
   <si>
@@ -121,16 +124,13 @@
     <t>MARC</t>
   </si>
   <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>FLAG:XAVIER // TAN DI ER // SYAFI'I</t>
+    <t>FLAG:TAN DI ER // XAVIER // KAH FAI</t>
   </si>
   <si>
     <t>LAST ENSURER: ANIQ</t>
   </si>
   <si>
-    <t>BREAKFAST:DHRUVA // DINNER:MARC</t>
+    <t>BREAKFAST:DHRUVA // DINNER:JUN</t>
   </si>
 </sst>
 </file>
@@ -191,13 +191,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,25 +209,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,15 +273,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,13 +291,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -672,28 +672,28 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="9"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -704,26 +704,26 @@
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="6"/>
       <c r="N5" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -734,26 +734,24 @@
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="4">
         <v>6</v>
       </c>
@@ -764,28 +762,30 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="4">
         <v>7</v>
       </c>
@@ -798,26 +798,28 @@
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4">
@@ -832,28 +834,28 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="6"/>
+      <c r="L13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="11"/>
       <c r="N13" s="4">
         <v>7</v>
       </c>
@@ -864,32 +866,32 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="K15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="8"/>
+      <c r="L15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="10"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -900,22 +902,22 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
       <c r="N17" s="4">
         <v>0</v>
       </c>
@@ -926,22 +928,22 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="B19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="4">
         <v>0</v>
       </c>
@@ -952,30 +954,30 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="4">
         <v>6</v>
       </c>
@@ -986,32 +988,32 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="E23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="8"/>
       <c r="N23" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1020,34 +1022,32 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="9" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M25" s="12"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1107,14 +1107,13 @@
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
     <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="L13:M13"/>
@@ -1123,7 +1122,8 @@
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>
     <mergeCell ref="D26:J28"/>

</xml_diff>

<commit_message>
Minimum viable prototype of desktop app
Still need to fix some bugs as highlighted in previous commits
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 060824 TUESDAY</t>
+    <t>DUTY 110824 SUNDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -61,45 +61,45 @@
     <t>HAKIM</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>DESK</t>
+  </si>
+  <si>
     <t>SENTRY</t>
   </si>
   <si>
-    <t>IN</t>
+    <t>XAVIER</t>
   </si>
   <si>
     <t>X-RAY</t>
   </si>
   <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
     <t>OUT</t>
   </si>
   <si>
-    <t>XAVIER</t>
+    <t>TAN DI ER</t>
   </si>
   <si>
     <t>SCA1</t>
   </si>
   <si>
-    <t>KAH FAI</t>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>ANIQ</t>
+  </si>
+  <si>
+    <t>JUN</t>
   </si>
   <si>
     <t>SCA2</t>
   </si>
   <si>
-    <t>DESK</t>
-  </si>
-  <si>
-    <t>TAN DI ER</t>
-  </si>
-  <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
-    <t>JUN</t>
-  </si>
-  <si>
-    <t>PAC</t>
-  </si>
-  <si>
     <t>SYAFI'I</t>
   </si>
   <si>
@@ -124,13 +124,13 @@
     <t>MARC</t>
   </si>
   <si>
-    <t>FLAG:TAN DI ER // XAVIER // KAH FAI</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: ANIQ</t>
-  </si>
-  <si>
-    <t>BREAKFAST:DHRUVA // DINNER:JUN</t>
+    <t>FLAG:DHRUVA // HAKIM // SYAFI'I</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: XAVIER</t>
+  </si>
+  <si>
+    <t>BREAKFAST:ANIQ // DINNER:JUN</t>
   </si>
 </sst>
 </file>
@@ -191,13 +191,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,12 +216,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,12 +279,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,22 +676,20 @@
         <v>15</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="4">
         <v>6</v>
       </c>
@@ -702,28 +700,30 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="6"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
       <c r="N5" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -732,28 +732,32 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="J7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -762,30 +766,26 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="11"/>
       <c r="N9" s="4">
         <v>7</v>
       </c>
@@ -798,30 +798,28 @@
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6" t="s">
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="4"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="5"/>
       <c r="N11" s="4">
         <v>7</v>
       </c>
@@ -834,28 +832,28 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="11"/>
+      <c r="L13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="4"/>
       <c r="N13" s="4">
         <v>7</v>
       </c>
@@ -868,30 +866,30 @@
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="G15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="10"/>
+      <c r="K15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="9"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -956,28 +954,28 @@
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="10"/>
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
       <c r="N21" s="4">
         <v>6</v>
       </c>
@@ -990,30 +988,30 @@
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6" t="s">
+      <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1024,30 +1022,32 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="M25" s="6"/>
       <c r="N25" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1107,23 +1107,23 @@
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="L25:M25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>
     <mergeCell ref="D26:J28"/>

</xml_diff>

<commit_message>
Fixed minor bugs (part 2?) before rolling out first prototype
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 110824 SUNDAY</t>
+    <t>DUTY 250824 SUNDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -73,21 +73,21 @@
     <t>XAVIER</t>
   </si>
   <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>SCA1</t>
+  </si>
+  <si>
     <t>X-RAY</t>
   </si>
   <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
     <t>TAN DI ER</t>
   </si>
   <si>
-    <t>SCA1</t>
-  </si>
-  <si>
     <t>PAC</t>
   </si>
   <si>
@@ -97,40 +97,40 @@
     <t>JUN</t>
   </si>
   <si>
+    <t>SYAFI'I</t>
+  </si>
+  <si>
+    <t>JOSHUA</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>ANIISH</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>HILMI</t>
+  </si>
+  <si>
+    <t>DHRUVA</t>
+  </si>
+  <si>
+    <t>MARC</t>
+  </si>
+  <si>
     <t>SCA2</t>
   </si>
   <si>
-    <t>SYAFI'I</t>
-  </si>
-  <si>
-    <t>JOSHUA</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>ANIISH</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>HILMI</t>
-  </si>
-  <si>
-    <t>DHRUVA</t>
-  </si>
-  <si>
-    <t>MARC</t>
-  </si>
-  <si>
-    <t>FLAG:DHRUVA // HAKIM // SYAFI'I</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: XAVIER</t>
-  </si>
-  <si>
-    <t>BREAKFAST:ANIQ // DINNER:JUN</t>
+    <t>FLAG:DHRUVA // KAH FAI // XAVIER</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: DHRUVA</t>
+  </si>
+  <si>
+    <t>BREAKFAST:ANIQ // DINNER:MARC</t>
   </si>
 </sst>
 </file>
@@ -209,13 +209,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FF00FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,7 +715,7 @@
       <c r="H5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="8"/>
@@ -735,22 +735,20 @@
         <v>20</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="9"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="8"/>
       <c r="K7" s="7" t="s">
         <v>17</v>
       </c>
@@ -766,22 +764,24 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="8"/>
+      <c r="K9" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="L9" s="11" t="s">
         <v>24</v>
       </c>
@@ -799,27 +799,27 @@
         <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="H11" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M11" s="5"/>
+      <c r="J11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="10"/>
       <c r="N11" s="4">
         <v>7</v>
       </c>
@@ -833,27 +833,29 @@
         <v>26</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="H13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="5"/>
       <c r="N13" s="4">
         <v>7</v>
       </c>
@@ -864,32 +866,32 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="6"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -900,10 +902,10 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -926,10 +928,10 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -952,20 +954,20 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="E21" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>16</v>
@@ -986,25 +988,25 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="10"/>
       <c r="D23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="6" t="s">
-        <v>16</v>
+      <c r="G23" s="8"/>
+      <c r="H23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1020,32 +1022,30 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="6" t="s">
+      <c r="K25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M25" s="6"/>
+      <c r="L25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="4"/>
       <c r="N25" s="4">
         <v>7</v>
       </c>
@@ -1110,19 +1110,19 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="K7:M7"/>
-    <mergeCell ref="C9:D9"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C13:D13"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:C23"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>

</xml_diff>

<commit_message>
Updated README.md with the details and rationale of project
Yet to update timetable_scheduling.py with the changes to data structure in roles, colors in generate_excel
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
-    <t>DUTY 250824 SUNDAY</t>
+    <t>DUTY 120924 THURSDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -61,36 +61,36 @@
     <t>HAKIM</t>
   </si>
   <si>
+    <t>SCA1</t>
+  </si>
+  <si>
+    <t>SENTRY</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
     <t>IN</t>
   </si>
   <si>
     <t>DESK</t>
   </si>
   <si>
-    <t>SENTRY</t>
-  </si>
-  <si>
-    <t>XAVIER</t>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>X-RAY</t>
+  </si>
+  <si>
+    <t>TAN DI ER</t>
   </si>
   <si>
     <t>OUT</t>
   </si>
   <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>SCA1</t>
-  </si>
-  <si>
-    <t>X-RAY</t>
-  </si>
-  <si>
-    <t>TAN DI ER</t>
-  </si>
-  <si>
-    <t>PAC</t>
-  </si>
-  <si>
     <t>ANIQ</t>
   </si>
   <si>
@@ -118,19 +118,19 @@
     <t>DHRUVA</t>
   </si>
   <si>
+    <t>SCA2</t>
+  </si>
+  <si>
     <t>MARC</t>
   </si>
   <si>
-    <t>SCA2</t>
-  </si>
-  <si>
-    <t>FLAG:DHRUVA // KAH FAI // XAVIER</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: DHRUVA</t>
-  </si>
-  <si>
-    <t>BREAKFAST:ANIQ // DINNER:MARC</t>
+    <t>FLAG:DHRUVA // TAN DI ER // MARC</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: HILMI</t>
+  </si>
+  <si>
+    <t>BREAKFAST:JUN // DINNER:ANIQ</t>
   </si>
 </sst>
 </file>
@@ -191,6 +191,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -203,25 +221,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,6 +273,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,9 +285,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -672,26 +672,26 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -702,26 +702,24 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6" t="s">
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="4">
         <v>6</v>
       </c>
@@ -732,25 +730,27 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="8"/>
+      <c r="G7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="8"/>
       <c r="K7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -766,28 +766,28 @@
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="11" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -798,28 +798,30 @@
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="10" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="10"/>
+      <c r="L11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="4"/>
       <c r="N11" s="4">
         <v>7</v>
       </c>
@@ -832,32 +834,30 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="4" t="s">
+      <c r="E13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -868,30 +868,30 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="10" t="s">
+      <c r="G15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="6"/>
+      <c r="M15" s="11"/>
       <c r="N15" s="4">
         <v>7</v>
       </c>
@@ -956,28 +956,28 @@
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6"/>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10"/>
       <c r="D21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="4">
         <v>6</v>
       </c>
@@ -990,30 +990,30 @@
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="K23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="10"/>
       <c r="N23" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1022,30 +1022,30 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="4" t="s">
+      <c r="B25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="9"/>
       <c r="N25" s="4">
         <v>7</v>
       </c>
@@ -1107,22 +1107,22 @@
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="K7:M7"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="A26:C28"/>
     <mergeCell ref="K26:N28"/>

</xml_diff>